<commit_message>
wip plan de formation et plan mise ne place Leavitt Diamant
</commit_message>
<xml_diff>
--- a/Phase-1-preparation/Training_plans/training_plans.xlsx
+++ b/Phase-1-preparation/Training_plans/training_plans.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelkonrath/Documents/Epitech/ProjetMSC1/Gotham/gotham_2020_20/Phase-1-preparation/Training_plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91389F0-791C-AB4A-B61B-2239CDF93F9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD312A9-37BF-F044-8ABF-36C7A510615F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4BC05C21-79CF-024B-B5FB-93BFA457E75A}"/>
+    <workbookView xWindow="7740" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4BC05C21-79CF-024B-B5FB-93BFA457E75A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Training plans" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>Training plans</t>
   </si>
@@ -150,6 +150,120 @@
   </si>
   <si>
     <t>The IT egenieer referent for the time manager app</t>
+  </si>
+  <si>
+    <t>2 - Trucks with GPS</t>
+  </si>
+  <si>
+    <t>Team managers</t>
+  </si>
+  <si>
+    <t>get truck location, how to identify a truck</t>
+  </si>
+  <si>
+    <t>Team manager referent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">advance gps settings, </t>
+  </si>
+  <si>
+    <t>All team manager department</t>
+  </si>
+  <si>
+    <t>Team manager referent 1</t>
+  </si>
+  <si>
+    <t>Truck's driver</t>
+  </si>
+  <si>
+    <t>Check gps on, how to turn on off, how to repport a malfunction to the maintenance team</t>
+  </si>
+  <si>
+    <t>All truck's driver</t>
+  </si>
+  <si>
+    <t>Mainteance department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to install a gps on truck </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT department </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check truck's location </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All It department </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All maintenance department </t>
+  </si>
+  <si>
+    <t>3 - Employees equip with eletronic device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic presentation </t>
+  </si>
+  <si>
+    <t>IT new recrue</t>
+  </si>
+  <si>
+    <t>Basic entreprise onboarding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How execute preventive and currative maintenance plan </t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>Technical assistance posture</t>
+  </si>
+  <si>
+    <t>4 - Deploy drones to monitor the street cleenliness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drone pilot </t>
+  </si>
+  <si>
+    <t>how to define a good flight plan</t>
+  </si>
+  <si>
+    <t>pilots + team manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report anomaly procedure </t>
+  </si>
+  <si>
+    <t>maintenance Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolve basic failure on drones </t>
+  </si>
+  <si>
+    <t>maintenance Department Referent</t>
+  </si>
+  <si>
+    <t>Definition of a maintenance procedure with supplier / after sales service for serious breakdowns</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>2 pilots</t>
+  </si>
+  <si>
+    <t>2 pilots and 1 team manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all maintenance department </t>
+  </si>
+  <si>
+    <t>Maintenance departmenet referent</t>
   </si>
 </sst>
 </file>
@@ -196,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +335,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3A8FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -243,16 +369,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -260,6 +401,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF3A8FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -568,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADFC04F-6AAC-444C-AB05-143CAA0D0B63}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,13 +730,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -598,19 +744,19 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -627,13 +773,13 @@
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -721,22 +867,226 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="11" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
maj impact des changement sur lentreprise
</commit_message>
<xml_diff>
--- a/Phase-1-preparation/Training_plans/training_plans.xlsx
+++ b/Phase-1-preparation/Training_plans/training_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelkonrath/Documents/Epitech/ProjetMSC1/Gotham/gotham_2020_20/Phase-1-preparation/Training_plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD312A9-37BF-F044-8ABF-36C7A510615F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F6C8B-0B55-E845-BEBB-8F3DFFF0ACA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4BC05C21-79CF-024B-B5FB-93BFA457E75A}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4BC05C21-79CF-024B-B5FB-93BFA457E75A}"/>
   </bookViews>
   <sheets>
     <sheet name="Training plans" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
   <si>
     <t>Training plans</t>
   </si>
@@ -155,6 +155,9 @@
     <t>2 - Trucks with GPS</t>
   </si>
   <si>
+    <t xml:space="preserve">Team manager </t>
+  </si>
+  <si>
     <t>Team managers</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
     <t>Team manager referent 1</t>
   </si>
   <si>
+    <t>truck's driver</t>
+  </si>
+  <si>
     <t>Truck's driver</t>
   </si>
   <si>
@@ -264,6 +270,18 @@
   </si>
   <si>
     <t>Maintenance departmenet referent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 - Change citizen's trashes </t>
+  </si>
+  <si>
+    <t>Get information from trashes sensors</t>
+  </si>
+  <si>
+    <t>Adapte garbage collector's route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get notification of changing route </t>
   </si>
 </sst>
 </file>
@@ -360,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -394,6 +412,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,15 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADFC04F-6AAC-444C-AB05-143CAA0D0B63}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="45.1640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
@@ -872,87 +896,87 @@
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>22</v>
@@ -964,124 +988,168 @@
     <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="9"/>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="11" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A10:A14"/>

</xml_diff>